<commit_message>
Corrected stick force measurement
</commit_message>
<xml_diff>
--- a/Post_Flight_Datasheet_13_03_V2.xlsx
+++ b/Post_Flight_Datasheet_13_03_V2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\PycharmProjects\SVV_assignment\FD_assignment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC7CF49-4C95-4075-A9B1-97078357A8CB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="1080" yWindow="-108" windowWidth="22068" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -226,7 +232,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
@@ -273,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
@@ -290,7 +296,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -390,7 +396,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -672,36 +684,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3"/>
-    <col min="2" max="2" width="8.140625"/>
+    <col min="2" max="2" width="8.109375"/>
     <col min="3" max="3" width="7"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="7"/>
-    <col min="14" max="1025" width="8.5703125"/>
+    <col min="14" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -713,7 +725,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -725,13 +737,13 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>6</v>
       </c>
@@ -739,7 +751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -750,7 +762,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -761,7 +773,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -772,7 +784,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -783,7 +795,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -794,7 +806,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -805,7 +817,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -816,7 +828,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -827,7 +839,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -838,7 +850,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -846,12 +858,12 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -859,7 +871,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -891,7 +903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
@@ -920,7 +932,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -957,7 +969,7 @@
         <v>-18.100000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>-21.216666666666665</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1031,7 +1043,7 @@
         <v>-23.5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1068,7 +1080,7 @@
         <v>-25.55</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1105,7 +1117,7 @@
         <v>-27.5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1142,7 +1154,7 @@
         <v>-28.066666666666663</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
@@ -1156,23 +1168,23 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>41</v>
       </c>
       <c r="E39" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -1204,7 +1216,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
         <v>42</v>
       </c>
@@ -1233,7 +1245,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1247,7 +1259,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1261,7 +1273,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>3</v>
       </c>
@@ -1275,7 +1287,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4</v>
       </c>
@@ -1289,7 +1301,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>5</v>
       </c>
@@ -1303,7 +1315,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>6</v>
       </c>
@@ -1317,7 +1329,7 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>7</v>
       </c>
@@ -1331,17 +1343,17 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1349,7 +1361,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -1390,7 +1402,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
         <v>42</v>
       </c>
@@ -1428,7 +1440,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1</v>
       </c>
@@ -1467,7 +1479,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2</v>
       </c>
@@ -1506,7 +1518,7 @@
         <v>-3.2</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>3</v>
       </c>
@@ -1545,7 +1557,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>4</v>
       </c>
@@ -1569,7 +1581,7 @@
         <v>3.8</v>
       </c>
       <c r="I62" s="2">
-        <v>-15.5</v>
+        <v>15.5</v>
       </c>
       <c r="J62" s="2">
         <v>467.5</v>
@@ -1584,7 +1596,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>5</v>
       </c>
@@ -1601,7 +1613,7 @@
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>6</v>
       </c>
@@ -1618,7 +1630,7 @@
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>7</v>
       </c>
@@ -1635,23 +1647,23 @@
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>49</v>
       </c>
       <c r="C70" s="2"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>50</v>
       </c>
@@ -1661,7 +1673,7 @@
       </c>
       <c r="H71" s="2"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>21</v>
       </c>
@@ -1702,7 +1714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
         <v>42</v>
       </c>
@@ -1740,7 +1752,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1</v>
       </c>
@@ -1779,7 +1791,7 @@
         <v>-5.2</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2</v>
       </c>
@@ -1818,17 +1830,17 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
         <v>53</v>
       </c>
@@ -1839,7 +1851,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
         <v>42</v>
       </c>
@@ -1850,7 +1862,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>54</v>
       </c>
@@ -1870,7 +1882,7 @@
         <v>4.5000000000000005E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>57</v>
       </c>

</xml_diff>